<commit_message>
Updated contribution sheet to use template
</commit_message>
<xml_diff>
--- a/contribution/contributions-summary-by-a1720458.xlsx
+++ b/contribution/contributions-summary-by-a1720458.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\Year Three\ESASI\Assignment\esas-senate-voting-system\assessments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\Year Three\ESASI\Assignment\esas-senate-voting-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F87AFD40-F8BA-4189-B03A-283F1A11B413}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7DEA9D-E47F-4997-B9C6-18120306A708}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="4170" windowWidth="15600" windowHeight="18990" xr2:uid="{E041243A-779A-43B5-97DC-DF565D594CAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{2C0029F1-931C-FB40-B057-6910B2A1CD93}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Contributions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,57 +30,140 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Member's Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+  <si>
+    <t>Contributions Assessed by:</t>
+  </si>
+  <si>
+    <t>Group:</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t>Contribution</t>
   </si>
   <si>
-    <t>Suggested Grade</t>
-  </si>
-  <si>
-    <t>Max Verhagen</t>
-  </si>
-  <si>
-    <t>Dan Bruer</t>
-  </si>
-  <si>
-    <t>Alfred Chen</t>
-  </si>
-  <si>
-    <t>Aiman Asyraaf</t>
-  </si>
-  <si>
-    <t>Good amout</t>
-  </si>
-  <si>
-    <t>Good amount</t>
-  </si>
-  <si>
-    <t>Good initiative</t>
-  </si>
-  <si>
-    <t>No contribution</t>
-  </si>
-  <si>
-    <t>A+</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Contribution grades should be entered as one of the following</t>
+  </si>
+  <si>
+    <t>Higher Distinction</t>
+  </si>
+  <si>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>Distinction</t>
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Zero</t>
+  </si>
+  <si>
+    <t>Iteration 1</t>
+  </si>
+  <si>
+    <t>Iteration 2</t>
+  </si>
+  <si>
+    <t>Iteration 3</t>
+  </si>
+  <si>
+    <t>Iteration 4</t>
+  </si>
+  <si>
+    <t>a1702065</t>
+  </si>
+  <si>
+    <t>Group 09</t>
+  </si>
+  <si>
+    <t>Dan</t>
+  </si>
+  <si>
+    <t>Parthey</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Xuxin</t>
+  </si>
+  <si>
+    <t>Aiman</t>
+  </si>
+  <si>
+    <t>a1720458</t>
+  </si>
+  <si>
+    <t>Parthey Bhatt</t>
+  </si>
+  <si>
+    <t>a1724402</t>
+  </si>
+  <si>
+    <t>Good initiative to pick up reasonable amount of work and attempting to complete it</t>
+  </si>
+  <si>
+    <t>Setup for framework and completed use cases</t>
+  </si>
+  <si>
+    <t>Great communication and wanting to help organize the project. Good work on assigned work.</t>
+  </si>
+  <si>
+    <t>Kept up with team members and tried to work on prject even with the illness</t>
+  </si>
+  <si>
+    <t>a1725532</t>
+  </si>
+  <si>
+    <t>a1732609</t>
+  </si>
+  <si>
+    <t>No communication with team members</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -95,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -103,12 +186,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,76 +593,443 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E60444-DA89-4DBA-BF48-5171DA06B411}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1123791F-6216-E444-80F3-ACD6A6EE1C15}">
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="81" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="str">
+        <f>A6</f>
+        <v>a1724402</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f>B6</f>
+        <v>Dan</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="str">
+        <f t="shared" ref="A15:B15" si="0">A7</f>
+        <v>a1720458</v>
+      </c>
+      <c r="B15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Parthey</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="str">
+        <f t="shared" ref="A16:B16" si="1">A8</f>
+        <v>a1725532</v>
+      </c>
+      <c r="B16" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>Max</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="str">
+        <f t="shared" ref="A17:B17" si="2">A9</f>
+        <v>a1702065</v>
+      </c>
+      <c r="B17" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>Xuxin</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="str">
+        <f t="shared" ref="A18:B18" si="3">A10</f>
+        <v>a1732609</v>
+      </c>
+      <c r="B18" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>Aiman</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="str">
+        <f t="shared" ref="A22:B22" si="4">A14</f>
+        <v>a1724402</v>
+      </c>
+      <c r="B22" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>Dan</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="str">
+        <f t="shared" ref="A23:B23" si="5">A15</f>
+        <v>a1720458</v>
+      </c>
+      <c r="B23" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>Parthey</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="str">
+        <f t="shared" ref="A24:B24" si="6">A16</f>
+        <v>a1725532</v>
+      </c>
+      <c r="B24" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>Max</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="str">
+        <f t="shared" ref="A25:B25" si="7">A17</f>
+        <v>a1702065</v>
+      </c>
+      <c r="B25" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v>Xuxin</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="str">
+        <f t="shared" ref="A26:B26" si="8">A18</f>
+        <v>a1732609</v>
+      </c>
+      <c r="B26" s="13" t="str">
+        <f t="shared" si="8"/>
+        <v>Aiman</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="str">
+        <f t="shared" ref="A30:B30" si="9">A22</f>
+        <v>a1724402</v>
+      </c>
+      <c r="B30" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v>Dan</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="str">
+        <f t="shared" ref="A31:B31" si="10">A23</f>
+        <v>a1720458</v>
+      </c>
+      <c r="B31" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v>Parthey</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="str">
+        <f t="shared" ref="A32:B32" si="11">A24</f>
+        <v>a1725532</v>
+      </c>
+      <c r="B32" s="9" t="str">
+        <f t="shared" si="11"/>
+        <v>Max</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="str">
+        <f t="shared" ref="A33:B33" si="12">A25</f>
+        <v>a1702065</v>
+      </c>
+      <c r="B33" s="9" t="str">
+        <f t="shared" si="12"/>
+        <v>Xuxin</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="str">
+        <f t="shared" ref="A34:B34" si="13">A26</f>
+        <v>a1732609</v>
+      </c>
+      <c r="B34" s="13" t="str">
+        <f t="shared" si="13"/>
+        <v>Aiman</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C37" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C39" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="16">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated contirbution sheet by parthey for week 2 iteration
</commit_message>
<xml_diff>
--- a/contribution/contributions-summary-by-a1720458.xlsx
+++ b/contribution/contributions-summary-by-a1720458.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\Year Three\ESASI\Assignment\esas-senate-voting-system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\Year Three\ESASI\Assignment\esas-senate-voting-system\assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7DEA9D-E47F-4997-B9C6-18120306A708}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC3B1C3-4E6F-4803-8EAE-9F95E80B452A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{2C0029F1-931C-FB40-B057-6910B2A1CD93}"/>
+    <workbookView xWindow="-15480" yWindow="4170" windowWidth="15600" windowHeight="18990" xr2:uid="{2C0029F1-931C-FB40-B057-6910B2A1CD93}"/>
   </bookViews>
   <sheets>
     <sheet name="Contributions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Contributions Assessed by:</t>
   </si>
@@ -147,6 +147,21 @@
   </si>
   <si>
     <t>No communication with team members</t>
+  </si>
+  <si>
+    <t>Good work on given user story tasks producing tests and functionality.</t>
+  </si>
+  <si>
+    <t>Keeping the team motivated, assigning work to individual members. Good work on the admin page.</t>
+  </si>
+  <si>
+    <t>Good work on creating adding and deleting functionality for parties and candidates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazing work on the frontend side of voting page. </t>
+  </si>
+  <si>
+    <t>Some commitment to work in a group but no visible work done yet.</t>
   </si>
 </sst>
 </file>
@@ -596,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1123791F-6216-E444-80F3-ACD6A6EE1C15}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -754,10 +769,14 @@
         <f>B6</f>
         <v>Dan</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f t="shared" ref="A15:B15" si="0">A7</f>
         <v>a1720458</v>
@@ -766,8 +785,12 @@
         <f t="shared" si="0"/>
         <v>Parthey</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
+      <c r="C15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
@@ -778,8 +801,12 @@
         <f t="shared" si="1"/>
         <v>Max</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
@@ -790,8 +817,12 @@
         <f t="shared" si="2"/>
         <v>Xuxin</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="str">
@@ -802,8 +833,12 @@
         <f t="shared" si="3"/>
         <v>Aiman</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
+      <c r="C18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>

</xml_diff>